<commit_message>
Updated predict today to change confidence levels
</commit_message>
<xml_diff>
--- a/current_season_games.xlsx
+++ b/current_season_games.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nboys\College Basketball Model\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7AE2D4FD-ED94-4CA5-9484-D38893EDA1C9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5394A9B2-F814-427E-A6B7-79CA6A7F04EC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-96" yWindow="-96" windowWidth="20928" windowHeight="12432" xr2:uid="{29496817-D00E-4FC1-8AE8-A830BE9E34D8}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4908" uniqueCount="1384">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5108" uniqueCount="1418">
   <si>
     <t>Date</t>
   </si>
@@ -4188,6 +4188,108 @@
   </si>
   <si>
     <t>94-85</t>
+  </si>
+  <si>
+    <t>93-80</t>
+  </si>
+  <si>
+    <t>80-93</t>
+  </si>
+  <si>
+    <t>91-66</t>
+  </si>
+  <si>
+    <t>66-91</t>
+  </si>
+  <si>
+    <t>92-85</t>
+  </si>
+  <si>
+    <t>85-92</t>
+  </si>
+  <si>
+    <t>93-50</t>
+  </si>
+  <si>
+    <t>50-93</t>
+  </si>
+  <si>
+    <t>74-68</t>
+  </si>
+  <si>
+    <t>68-74</t>
+  </si>
+  <si>
+    <t>69-72</t>
+  </si>
+  <si>
+    <t>72-69</t>
+  </si>
+  <si>
+    <t>87-57</t>
+  </si>
+  <si>
+    <t>57-87</t>
+  </si>
+  <si>
+    <t>75-62</t>
+  </si>
+  <si>
+    <t>62-75</t>
+  </si>
+  <si>
+    <t>94-66</t>
+  </si>
+  <si>
+    <t>66-94</t>
+  </si>
+  <si>
+    <t>96-57</t>
+  </si>
+  <si>
+    <t>57-96</t>
+  </si>
+  <si>
+    <t>84-83</t>
+  </si>
+  <si>
+    <t>83-84</t>
+  </si>
+  <si>
+    <t>81-59</t>
+  </si>
+  <si>
+    <t>59-81</t>
+  </si>
+  <si>
+    <t>84-50</t>
+  </si>
+  <si>
+    <t>50-84</t>
+  </si>
+  <si>
+    <t>122-50</t>
+  </si>
+  <si>
+    <t>50-122</t>
+  </si>
+  <si>
+    <t>94-69</t>
+  </si>
+  <si>
+    <t>69-94</t>
+  </si>
+  <si>
+    <t>62-71</t>
+  </si>
+  <si>
+    <t>71-62</t>
+  </si>
+  <si>
+    <t>66-79</t>
+  </si>
+  <si>
+    <t>79-66</t>
   </si>
 </sst>
 </file>
@@ -4647,10 +4749,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FD64AC2A-6E85-4C33-B675-E7FA9CCF4CBE}">
-  <dimension ref="A1:L1225"/>
+  <dimension ref="A1:L1275"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A1155" workbookViewId="0">
-      <selection activeCell="D1165" sqref="D1165"/>
+    <sheetView tabSelected="1" topLeftCell="A1221" workbookViewId="0">
+      <selection activeCell="A1226" sqref="A1226:L1275"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -50958,6 +51060,1906 @@
         <v>21.5</v>
       </c>
     </row>
+    <row r="1226" spans="1:12" ht="16.2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A1226" s="9">
+        <v>45978</v>
+      </c>
+      <c r="B1226" s="10" t="s">
+        <v>517</v>
+      </c>
+      <c r="C1226" s="10" t="s">
+        <v>59</v>
+      </c>
+      <c r="D1226" s="11" t="s">
+        <v>25</v>
+      </c>
+      <c r="E1226" s="11">
+        <v>-7.5</v>
+      </c>
+      <c r="F1226" s="11">
+        <v>141.5</v>
+      </c>
+      <c r="G1226" s="11">
+        <v>-345</v>
+      </c>
+      <c r="H1226" s="11" t="s">
+        <v>1384</v>
+      </c>
+      <c r="I1226" s="11">
+        <v>13</v>
+      </c>
+      <c r="J1226" s="11">
+        <v>5.5</v>
+      </c>
+      <c r="K1226" s="11">
+        <v>173</v>
+      </c>
+      <c r="L1226" s="11">
+        <v>31.5</v>
+      </c>
+    </row>
+    <row r="1227" spans="1:12" ht="16.2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A1227" s="12">
+        <v>45978</v>
+      </c>
+      <c r="B1227" s="13" t="s">
+        <v>59</v>
+      </c>
+      <c r="C1227" s="13" t="s">
+        <v>517</v>
+      </c>
+      <c r="D1227" s="14" t="s">
+        <v>23</v>
+      </c>
+      <c r="E1227" s="14">
+        <v>7.5</v>
+      </c>
+      <c r="F1227" s="14">
+        <v>141.5</v>
+      </c>
+      <c r="G1227" s="14">
+        <v>278</v>
+      </c>
+      <c r="H1227" s="14" t="s">
+        <v>1385</v>
+      </c>
+      <c r="I1227" s="14">
+        <v>-13</v>
+      </c>
+      <c r="J1227" s="14">
+        <v>-5.5</v>
+      </c>
+      <c r="K1227" s="14">
+        <v>173</v>
+      </c>
+      <c r="L1227" s="14">
+        <v>31.5</v>
+      </c>
+    </row>
+    <row r="1228" spans="1:12" ht="16.2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A1228" s="9">
+        <v>45978</v>
+      </c>
+      <c r="B1228" s="10" t="s">
+        <v>96</v>
+      </c>
+      <c r="C1228" s="10" t="s">
+        <v>556</v>
+      </c>
+      <c r="D1228" s="11" t="s">
+        <v>25</v>
+      </c>
+      <c r="E1228" s="11">
+        <v>-25.5</v>
+      </c>
+      <c r="F1228" s="11">
+        <v>144.5</v>
+      </c>
+      <c r="G1228" s="11">
+        <v>-9000</v>
+      </c>
+      <c r="H1228" s="11" t="s">
+        <v>1111</v>
+      </c>
+      <c r="I1228" s="11">
+        <v>20</v>
+      </c>
+      <c r="J1228" s="11">
+        <v>-5.5</v>
+      </c>
+      <c r="K1228" s="11">
+        <v>142</v>
+      </c>
+      <c r="L1228" s="11">
+        <v>-2.5</v>
+      </c>
+    </row>
+    <row r="1229" spans="1:12" ht="16.2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A1229" s="12">
+        <v>45978</v>
+      </c>
+      <c r="B1229" s="13" t="s">
+        <v>556</v>
+      </c>
+      <c r="C1229" s="13" t="s">
+        <v>96</v>
+      </c>
+      <c r="D1229" s="14" t="s">
+        <v>23</v>
+      </c>
+      <c r="E1229" s="14">
+        <v>25.5</v>
+      </c>
+      <c r="F1229" s="14">
+        <v>144.5</v>
+      </c>
+      <c r="G1229" s="14">
+        <v>2500</v>
+      </c>
+      <c r="H1229" s="14" t="s">
+        <v>1110</v>
+      </c>
+      <c r="I1229" s="14">
+        <v>-20</v>
+      </c>
+      <c r="J1229" s="14">
+        <v>5.5</v>
+      </c>
+      <c r="K1229" s="14">
+        <v>142</v>
+      </c>
+      <c r="L1229" s="14">
+        <v>-2.5</v>
+      </c>
+    </row>
+    <row r="1230" spans="1:12" ht="16.2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A1230" s="9">
+        <v>45978</v>
+      </c>
+      <c r="B1230" s="10" t="s">
+        <v>200</v>
+      </c>
+      <c r="C1230" s="10" t="s">
+        <v>652</v>
+      </c>
+      <c r="D1230" s="11" t="s">
+        <v>25</v>
+      </c>
+      <c r="E1230" s="11">
+        <v>-26</v>
+      </c>
+      <c r="F1230" s="11">
+        <v>143.5</v>
+      </c>
+      <c r="G1230" s="11">
+        <v>-6500</v>
+      </c>
+      <c r="H1230" s="11" t="s">
+        <v>1386</v>
+      </c>
+      <c r="I1230" s="11">
+        <v>25</v>
+      </c>
+      <c r="J1230" s="11">
+        <v>-1</v>
+      </c>
+      <c r="K1230" s="11">
+        <v>157</v>
+      </c>
+      <c r="L1230" s="11">
+        <v>13.5</v>
+      </c>
+    </row>
+    <row r="1231" spans="1:12" ht="16.2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A1231" s="12">
+        <v>45978</v>
+      </c>
+      <c r="B1231" s="13" t="s">
+        <v>652</v>
+      </c>
+      <c r="C1231" s="13" t="s">
+        <v>200</v>
+      </c>
+      <c r="D1231" s="14" t="s">
+        <v>23</v>
+      </c>
+      <c r="E1231" s="14">
+        <v>26</v>
+      </c>
+      <c r="F1231" s="14">
+        <v>143.5</v>
+      </c>
+      <c r="G1231" s="14">
+        <v>2000</v>
+      </c>
+      <c r="H1231" s="14" t="s">
+        <v>1387</v>
+      </c>
+      <c r="I1231" s="14">
+        <v>-25</v>
+      </c>
+      <c r="J1231" s="14">
+        <v>1</v>
+      </c>
+      <c r="K1231" s="14">
+        <v>157</v>
+      </c>
+      <c r="L1231" s="14">
+        <v>13.5</v>
+      </c>
+    </row>
+    <row r="1232" spans="1:12" ht="16.2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A1232" s="9">
+        <v>45978</v>
+      </c>
+      <c r="B1232" s="10" t="s">
+        <v>431</v>
+      </c>
+      <c r="C1232" s="10" t="s">
+        <v>674</v>
+      </c>
+      <c r="D1232" s="11" t="s">
+        <v>25</v>
+      </c>
+      <c r="E1232" s="11">
+        <v>-1.5</v>
+      </c>
+      <c r="F1232" s="11">
+        <v>153.5</v>
+      </c>
+      <c r="G1232" s="11">
+        <v>-121</v>
+      </c>
+      <c r="H1232" s="11" t="s">
+        <v>1388</v>
+      </c>
+      <c r="I1232" s="11">
+        <v>7</v>
+      </c>
+      <c r="J1232" s="11">
+        <v>5.5</v>
+      </c>
+      <c r="K1232" s="11">
+        <v>177</v>
+      </c>
+      <c r="L1232" s="11">
+        <v>23.5</v>
+      </c>
+    </row>
+    <row r="1233" spans="1:12" ht="16.2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A1233" s="12">
+        <v>45978</v>
+      </c>
+      <c r="B1233" s="13" t="s">
+        <v>674</v>
+      </c>
+      <c r="C1233" s="13" t="s">
+        <v>431</v>
+      </c>
+      <c r="D1233" s="14" t="s">
+        <v>23</v>
+      </c>
+      <c r="E1233" s="14">
+        <v>1.5</v>
+      </c>
+      <c r="F1233" s="14">
+        <v>153.5</v>
+      </c>
+      <c r="G1233" s="14">
+        <v>101</v>
+      </c>
+      <c r="H1233" s="14" t="s">
+        <v>1389</v>
+      </c>
+      <c r="I1233" s="14">
+        <v>-7</v>
+      </c>
+      <c r="J1233" s="14">
+        <v>-5.5</v>
+      </c>
+      <c r="K1233" s="14">
+        <v>177</v>
+      </c>
+      <c r="L1233" s="14">
+        <v>23.5</v>
+      </c>
+    </row>
+    <row r="1234" spans="1:12" ht="16.2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A1234" s="9">
+        <v>45978</v>
+      </c>
+      <c r="B1234" s="10" t="s">
+        <v>923</v>
+      </c>
+      <c r="C1234" s="10" t="s">
+        <v>356</v>
+      </c>
+      <c r="D1234" s="11" t="s">
+        <v>25</v>
+      </c>
+      <c r="E1234" s="11">
+        <v>5.5</v>
+      </c>
+      <c r="F1234" s="11">
+        <v>162.5</v>
+      </c>
+      <c r="G1234" s="11">
+        <v>205</v>
+      </c>
+      <c r="H1234" s="11" t="s">
+        <v>615</v>
+      </c>
+      <c r="I1234" s="11">
+        <v>9</v>
+      </c>
+      <c r="J1234" s="11">
+        <v>14.5</v>
+      </c>
+      <c r="K1234" s="11">
+        <v>157</v>
+      </c>
+      <c r="L1234" s="11">
+        <v>-5.5</v>
+      </c>
+    </row>
+    <row r="1235" spans="1:12" ht="16.2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A1235" s="12">
+        <v>45978</v>
+      </c>
+      <c r="B1235" s="13" t="s">
+        <v>356</v>
+      </c>
+      <c r="C1235" s="13" t="s">
+        <v>923</v>
+      </c>
+      <c r="D1235" s="14" t="s">
+        <v>23</v>
+      </c>
+      <c r="E1235" s="14">
+        <v>-5.5</v>
+      </c>
+      <c r="F1235" s="14">
+        <v>162.5</v>
+      </c>
+      <c r="G1235" s="14">
+        <v>-250</v>
+      </c>
+      <c r="H1235" s="14" t="s">
+        <v>614</v>
+      </c>
+      <c r="I1235" s="14">
+        <v>-9</v>
+      </c>
+      <c r="J1235" s="14">
+        <v>-14.5</v>
+      </c>
+      <c r="K1235" s="14">
+        <v>157</v>
+      </c>
+      <c r="L1235" s="14">
+        <v>-5.5</v>
+      </c>
+    </row>
+    <row r="1236" spans="1:12" ht="16.2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A1236" s="9">
+        <v>45978</v>
+      </c>
+      <c r="B1236" s="10" t="s">
+        <v>320</v>
+      </c>
+      <c r="C1236" s="10" t="s">
+        <v>83</v>
+      </c>
+      <c r="D1236" s="11" t="s">
+        <v>25</v>
+      </c>
+      <c r="E1236" s="11">
+        <v>-23.5</v>
+      </c>
+      <c r="F1236" s="11">
+        <v>151.5</v>
+      </c>
+      <c r="G1236" s="11">
+        <v>-6500</v>
+      </c>
+      <c r="H1236" s="11" t="s">
+        <v>1390</v>
+      </c>
+      <c r="I1236" s="11">
+        <v>43</v>
+      </c>
+      <c r="J1236" s="11">
+        <v>19.5</v>
+      </c>
+      <c r="K1236" s="11">
+        <v>143</v>
+      </c>
+      <c r="L1236" s="11">
+        <v>-8.5</v>
+      </c>
+    </row>
+    <row r="1237" spans="1:12" ht="16.2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A1237" s="12">
+        <v>45978</v>
+      </c>
+      <c r="B1237" s="13" t="s">
+        <v>83</v>
+      </c>
+      <c r="C1237" s="13" t="s">
+        <v>320</v>
+      </c>
+      <c r="D1237" s="14" t="s">
+        <v>23</v>
+      </c>
+      <c r="E1237" s="14">
+        <v>23.5</v>
+      </c>
+      <c r="F1237" s="14">
+        <v>151.5</v>
+      </c>
+      <c r="G1237" s="14">
+        <v>2000</v>
+      </c>
+      <c r="H1237" s="14" t="s">
+        <v>1391</v>
+      </c>
+      <c r="I1237" s="14">
+        <v>-43</v>
+      </c>
+      <c r="J1237" s="14">
+        <v>-19.5</v>
+      </c>
+      <c r="K1237" s="14">
+        <v>143</v>
+      </c>
+      <c r="L1237" s="14">
+        <v>-8.5</v>
+      </c>
+    </row>
+    <row r="1238" spans="1:12" ht="16.2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A1238" s="9">
+        <v>45978</v>
+      </c>
+      <c r="B1238" s="10" t="s">
+        <v>592</v>
+      </c>
+      <c r="C1238" s="10" t="s">
+        <v>363</v>
+      </c>
+      <c r="D1238" s="11" t="s">
+        <v>25</v>
+      </c>
+      <c r="E1238" s="11">
+        <v>-2</v>
+      </c>
+      <c r="F1238" s="11">
+        <v>138.5</v>
+      </c>
+      <c r="G1238" s="11">
+        <v>-135</v>
+      </c>
+      <c r="H1238" s="11" t="s">
+        <v>1392</v>
+      </c>
+      <c r="I1238" s="11">
+        <v>6</v>
+      </c>
+      <c r="J1238" s="11">
+        <v>4</v>
+      </c>
+      <c r="K1238" s="11">
+        <v>142</v>
+      </c>
+      <c r="L1238" s="11">
+        <v>3.5</v>
+      </c>
+    </row>
+    <row r="1239" spans="1:12" ht="16.2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A1239" s="12">
+        <v>45978</v>
+      </c>
+      <c r="B1239" s="13" t="s">
+        <v>363</v>
+      </c>
+      <c r="C1239" s="13" t="s">
+        <v>592</v>
+      </c>
+      <c r="D1239" s="14" t="s">
+        <v>23</v>
+      </c>
+      <c r="E1239" s="14">
+        <v>2</v>
+      </c>
+      <c r="F1239" s="14">
+        <v>138.5</v>
+      </c>
+      <c r="G1239" s="14">
+        <v>114</v>
+      </c>
+      <c r="H1239" s="14" t="s">
+        <v>1393</v>
+      </c>
+      <c r="I1239" s="14">
+        <v>-6</v>
+      </c>
+      <c r="J1239" s="14">
+        <v>-4</v>
+      </c>
+      <c r="K1239" s="14">
+        <v>142</v>
+      </c>
+      <c r="L1239" s="14">
+        <v>3.5</v>
+      </c>
+    </row>
+    <row r="1240" spans="1:12" ht="16.2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A1240" s="9">
+        <v>45978</v>
+      </c>
+      <c r="B1240" s="10" t="s">
+        <v>124</v>
+      </c>
+      <c r="C1240" s="10" t="s">
+        <v>176</v>
+      </c>
+      <c r="D1240" s="11" t="s">
+        <v>25</v>
+      </c>
+      <c r="E1240" s="11">
+        <v>-11.5</v>
+      </c>
+      <c r="F1240" s="11">
+        <v>164.5</v>
+      </c>
+      <c r="G1240" s="11">
+        <v>-850</v>
+      </c>
+      <c r="H1240" s="11" t="s">
+        <v>326</v>
+      </c>
+      <c r="I1240" s="11">
+        <v>6</v>
+      </c>
+      <c r="J1240" s="11">
+        <v>-5.5</v>
+      </c>
+      <c r="K1240" s="11">
+        <v>164</v>
+      </c>
+      <c r="L1240" s="11">
+        <v>-0.5</v>
+      </c>
+    </row>
+    <row r="1241" spans="1:12" ht="16.2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A1241" s="12">
+        <v>45978</v>
+      </c>
+      <c r="B1241" s="13" t="s">
+        <v>176</v>
+      </c>
+      <c r="C1241" s="13" t="s">
+        <v>124</v>
+      </c>
+      <c r="D1241" s="14" t="s">
+        <v>23</v>
+      </c>
+      <c r="E1241" s="14">
+        <v>11.5</v>
+      </c>
+      <c r="F1241" s="14">
+        <v>164.5</v>
+      </c>
+      <c r="G1241" s="14">
+        <v>575</v>
+      </c>
+      <c r="H1241" s="14" t="s">
+        <v>325</v>
+      </c>
+      <c r="I1241" s="14">
+        <v>-6</v>
+      </c>
+      <c r="J1241" s="14">
+        <v>5.5</v>
+      </c>
+      <c r="K1241" s="14">
+        <v>164</v>
+      </c>
+      <c r="L1241" s="14">
+        <v>-0.5</v>
+      </c>
+    </row>
+    <row r="1242" spans="1:12" ht="16.2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A1242" s="9">
+        <v>45978</v>
+      </c>
+      <c r="B1242" s="10" t="s">
+        <v>136</v>
+      </c>
+      <c r="C1242" s="10" t="s">
+        <v>257</v>
+      </c>
+      <c r="D1242" s="11" t="s">
+        <v>25</v>
+      </c>
+      <c r="E1242" s="11">
+        <v>-6.5</v>
+      </c>
+      <c r="F1242" s="11">
+        <v>145.5</v>
+      </c>
+      <c r="G1242" s="11">
+        <v>-290</v>
+      </c>
+      <c r="H1242" s="11" t="s">
+        <v>1394</v>
+      </c>
+      <c r="I1242" s="11">
+        <v>-3</v>
+      </c>
+      <c r="J1242" s="11">
+        <v>-9.5</v>
+      </c>
+      <c r="K1242" s="11">
+        <v>141</v>
+      </c>
+      <c r="L1242" s="11">
+        <v>-4.5</v>
+      </c>
+    </row>
+    <row r="1243" spans="1:12" ht="16.2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A1243" s="12">
+        <v>45978</v>
+      </c>
+      <c r="B1243" s="13" t="s">
+        <v>257</v>
+      </c>
+      <c r="C1243" s="13" t="s">
+        <v>136</v>
+      </c>
+      <c r="D1243" s="14" t="s">
+        <v>23</v>
+      </c>
+      <c r="E1243" s="14">
+        <v>6.5</v>
+      </c>
+      <c r="F1243" s="14">
+        <v>145.5</v>
+      </c>
+      <c r="G1243" s="14">
+        <v>235</v>
+      </c>
+      <c r="H1243" s="14" t="s">
+        <v>1395</v>
+      </c>
+      <c r="I1243" s="14">
+        <v>3</v>
+      </c>
+      <c r="J1243" s="14">
+        <v>9.5</v>
+      </c>
+      <c r="K1243" s="14">
+        <v>141</v>
+      </c>
+      <c r="L1243" s="14">
+        <v>-4.5</v>
+      </c>
+    </row>
+    <row r="1244" spans="1:12" ht="16.2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A1244" s="9">
+        <v>45978</v>
+      </c>
+      <c r="B1244" s="10" t="s">
+        <v>234</v>
+      </c>
+      <c r="C1244" s="10" t="s">
+        <v>395</v>
+      </c>
+      <c r="D1244" s="11" t="s">
+        <v>25</v>
+      </c>
+      <c r="E1244" s="11">
+        <v>-40</v>
+      </c>
+      <c r="F1244" s="11">
+        <v>170.5</v>
+      </c>
+      <c r="G1244" s="11">
+        <v>-10000</v>
+      </c>
+      <c r="H1244" s="11" t="s">
+        <v>1396</v>
+      </c>
+      <c r="I1244" s="11">
+        <v>30</v>
+      </c>
+      <c r="J1244" s="11">
+        <v>-10</v>
+      </c>
+      <c r="K1244" s="11">
+        <v>144</v>
+      </c>
+      <c r="L1244" s="11">
+        <v>-26.5</v>
+      </c>
+    </row>
+    <row r="1245" spans="1:12" ht="16.2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A1245" s="12">
+        <v>45978</v>
+      </c>
+      <c r="B1245" s="13" t="s">
+        <v>395</v>
+      </c>
+      <c r="C1245" s="13" t="s">
+        <v>234</v>
+      </c>
+      <c r="D1245" s="14" t="s">
+        <v>23</v>
+      </c>
+      <c r="E1245" s="14">
+        <v>40</v>
+      </c>
+      <c r="F1245" s="14">
+        <v>170.5</v>
+      </c>
+      <c r="G1245" s="14">
+        <v>3000</v>
+      </c>
+      <c r="H1245" s="14" t="s">
+        <v>1397</v>
+      </c>
+      <c r="I1245" s="14">
+        <v>-30</v>
+      </c>
+      <c r="J1245" s="14">
+        <v>10</v>
+      </c>
+      <c r="K1245" s="14">
+        <v>144</v>
+      </c>
+      <c r="L1245" s="14">
+        <v>-26.5</v>
+      </c>
+    </row>
+    <row r="1246" spans="1:12" ht="16.2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A1246" s="9">
+        <v>45978</v>
+      </c>
+      <c r="B1246" s="10" t="s">
+        <v>855</v>
+      </c>
+      <c r="C1246" s="10" t="s">
+        <v>519</v>
+      </c>
+      <c r="D1246" s="11" t="s">
+        <v>25</v>
+      </c>
+      <c r="E1246" s="11">
+        <v>-4</v>
+      </c>
+      <c r="F1246" s="11">
+        <v>145</v>
+      </c>
+      <c r="G1246" s="11">
+        <v>-185</v>
+      </c>
+      <c r="H1246" s="11" t="s">
+        <v>130</v>
+      </c>
+      <c r="I1246" s="11">
+        <v>-4</v>
+      </c>
+      <c r="J1246" s="11">
+        <v>-8</v>
+      </c>
+      <c r="K1246" s="11">
+        <v>152</v>
+      </c>
+      <c r="L1246" s="11">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1247" spans="1:12" ht="16.2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A1247" s="12">
+        <v>45978</v>
+      </c>
+      <c r="B1247" s="13" t="s">
+        <v>519</v>
+      </c>
+      <c r="C1247" s="13" t="s">
+        <v>855</v>
+      </c>
+      <c r="D1247" s="14" t="s">
+        <v>23</v>
+      </c>
+      <c r="E1247" s="14">
+        <v>4</v>
+      </c>
+      <c r="F1247" s="14">
+        <v>145</v>
+      </c>
+      <c r="G1247" s="14">
+        <v>161</v>
+      </c>
+      <c r="H1247" s="14" t="s">
+        <v>129</v>
+      </c>
+      <c r="I1247" s="14">
+        <v>4</v>
+      </c>
+      <c r="J1247" s="14">
+        <v>8</v>
+      </c>
+      <c r="K1247" s="14">
+        <v>152</v>
+      </c>
+      <c r="L1247" s="14">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1248" spans="1:12" ht="16.2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A1248" s="9">
+        <v>45978</v>
+      </c>
+      <c r="B1248" s="10" t="s">
+        <v>486</v>
+      </c>
+      <c r="C1248" s="10" t="s">
+        <v>327</v>
+      </c>
+      <c r="D1248" s="11" t="s">
+        <v>25</v>
+      </c>
+      <c r="E1248" s="11">
+        <v>-18.5</v>
+      </c>
+      <c r="F1248" s="11">
+        <v>145.5</v>
+      </c>
+      <c r="G1248" s="11">
+        <v>-3200</v>
+      </c>
+      <c r="H1248" s="11" t="s">
+        <v>1398</v>
+      </c>
+      <c r="I1248" s="11">
+        <v>13</v>
+      </c>
+      <c r="J1248" s="11">
+        <v>-5.5</v>
+      </c>
+      <c r="K1248" s="11">
+        <v>137</v>
+      </c>
+      <c r="L1248" s="11">
+        <v>-8.5</v>
+      </c>
+    </row>
+    <row r="1249" spans="1:12" ht="16.2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A1249" s="12">
+        <v>45978</v>
+      </c>
+      <c r="B1249" s="13" t="s">
+        <v>327</v>
+      </c>
+      <c r="C1249" s="13" t="s">
+        <v>486</v>
+      </c>
+      <c r="D1249" s="14" t="s">
+        <v>23</v>
+      </c>
+      <c r="E1249" s="14">
+        <v>18.5</v>
+      </c>
+      <c r="F1249" s="14">
+        <v>145.5</v>
+      </c>
+      <c r="G1249" s="14">
+        <v>1400</v>
+      </c>
+      <c r="H1249" s="14" t="s">
+        <v>1399</v>
+      </c>
+      <c r="I1249" s="14">
+        <v>-13</v>
+      </c>
+      <c r="J1249" s="14">
+        <v>5.5</v>
+      </c>
+      <c r="K1249" s="14">
+        <v>137</v>
+      </c>
+      <c r="L1249" s="14">
+        <v>-8.5</v>
+      </c>
+    </row>
+    <row r="1250" spans="1:12" ht="16.2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A1250" s="9">
+        <v>45978</v>
+      </c>
+      <c r="B1250" s="10" t="s">
+        <v>32</v>
+      </c>
+      <c r="C1250" s="10" t="s">
+        <v>655</v>
+      </c>
+      <c r="D1250" s="11" t="s">
+        <v>25</v>
+      </c>
+      <c r="E1250" s="11">
+        <v>-22.5</v>
+      </c>
+      <c r="F1250" s="11">
+        <v>157.5</v>
+      </c>
+      <c r="G1250" s="11">
+        <v>-5000</v>
+      </c>
+      <c r="H1250" s="11" t="s">
+        <v>1400</v>
+      </c>
+      <c r="I1250" s="11">
+        <v>28</v>
+      </c>
+      <c r="J1250" s="11">
+        <v>5.5</v>
+      </c>
+      <c r="K1250" s="11">
+        <v>160</v>
+      </c>
+      <c r="L1250" s="11">
+        <v>2.5</v>
+      </c>
+    </row>
+    <row r="1251" spans="1:12" ht="16.2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A1251" s="12">
+        <v>45978</v>
+      </c>
+      <c r="B1251" s="13" t="s">
+        <v>655</v>
+      </c>
+      <c r="C1251" s="13" t="s">
+        <v>32</v>
+      </c>
+      <c r="D1251" s="14" t="s">
+        <v>23</v>
+      </c>
+      <c r="E1251" s="14">
+        <v>22.5</v>
+      </c>
+      <c r="F1251" s="14">
+        <v>157.5</v>
+      </c>
+      <c r="G1251" s="14">
+        <v>1800</v>
+      </c>
+      <c r="H1251" s="14" t="s">
+        <v>1401</v>
+      </c>
+      <c r="I1251" s="14">
+        <v>-28</v>
+      </c>
+      <c r="J1251" s="14">
+        <v>-5.5</v>
+      </c>
+      <c r="K1251" s="14">
+        <v>160</v>
+      </c>
+      <c r="L1251" s="14">
+        <v>2.5</v>
+      </c>
+    </row>
+    <row r="1252" spans="1:12" ht="16.2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A1252" s="9">
+        <v>45978</v>
+      </c>
+      <c r="B1252" s="10" t="s">
+        <v>116</v>
+      </c>
+      <c r="C1252" s="10" t="s">
+        <v>658</v>
+      </c>
+      <c r="D1252" s="11" t="s">
+        <v>25</v>
+      </c>
+      <c r="E1252" s="11">
+        <v>-39</v>
+      </c>
+      <c r="F1252" s="11">
+        <v>146.5</v>
+      </c>
+      <c r="G1252" s="11">
+        <v>-10000</v>
+      </c>
+      <c r="H1252" s="11" t="s">
+        <v>1402</v>
+      </c>
+      <c r="I1252" s="11">
+        <v>39</v>
+      </c>
+      <c r="J1252" s="11">
+        <v>0</v>
+      </c>
+      <c r="K1252" s="11">
+        <v>153</v>
+      </c>
+      <c r="L1252" s="11">
+        <v>6.5</v>
+      </c>
+    </row>
+    <row r="1253" spans="1:12" ht="16.2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A1253" s="12">
+        <v>45978</v>
+      </c>
+      <c r="B1253" s="13" t="s">
+        <v>658</v>
+      </c>
+      <c r="C1253" s="13" t="s">
+        <v>116</v>
+      </c>
+      <c r="D1253" s="14" t="s">
+        <v>23</v>
+      </c>
+      <c r="E1253" s="14">
+        <v>39</v>
+      </c>
+      <c r="F1253" s="14">
+        <v>146.5</v>
+      </c>
+      <c r="G1253" s="14">
+        <v>3300</v>
+      </c>
+      <c r="H1253" s="14" t="s">
+        <v>1403</v>
+      </c>
+      <c r="I1253" s="14">
+        <v>-39</v>
+      </c>
+      <c r="J1253" s="14">
+        <v>0</v>
+      </c>
+      <c r="K1253" s="14">
+        <v>153</v>
+      </c>
+      <c r="L1253" s="14">
+        <v>6.5</v>
+      </c>
+    </row>
+    <row r="1254" spans="1:12" ht="16.2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A1254" s="9">
+        <v>45978</v>
+      </c>
+      <c r="B1254" s="10" t="s">
+        <v>482</v>
+      </c>
+      <c r="C1254" s="10" t="s">
+        <v>703</v>
+      </c>
+      <c r="D1254" s="11" t="s">
+        <v>25</v>
+      </c>
+      <c r="E1254" s="11">
+        <v>-12</v>
+      </c>
+      <c r="F1254" s="11">
+        <v>159.5</v>
+      </c>
+      <c r="G1254" s="11">
+        <v>-850</v>
+      </c>
+      <c r="H1254" s="11" t="s">
+        <v>1404</v>
+      </c>
+      <c r="I1254" s="11">
+        <v>1</v>
+      </c>
+      <c r="J1254" s="11">
+        <v>-11</v>
+      </c>
+      <c r="K1254" s="11">
+        <v>167</v>
+      </c>
+      <c r="L1254" s="11">
+        <v>7.5</v>
+      </c>
+    </row>
+    <row r="1255" spans="1:12" ht="16.2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A1255" s="12">
+        <v>45978</v>
+      </c>
+      <c r="B1255" s="13" t="s">
+        <v>703</v>
+      </c>
+      <c r="C1255" s="13" t="s">
+        <v>482</v>
+      </c>
+      <c r="D1255" s="14" t="s">
+        <v>23</v>
+      </c>
+      <c r="E1255" s="14">
+        <v>12</v>
+      </c>
+      <c r="F1255" s="14">
+        <v>159.5</v>
+      </c>
+      <c r="G1255" s="14">
+        <v>575</v>
+      </c>
+      <c r="H1255" s="14" t="s">
+        <v>1405</v>
+      </c>
+      <c r="I1255" s="14">
+        <v>-1</v>
+      </c>
+      <c r="J1255" s="14">
+        <v>11</v>
+      </c>
+      <c r="K1255" s="14">
+        <v>167</v>
+      </c>
+      <c r="L1255" s="14">
+        <v>7.5</v>
+      </c>
+    </row>
+    <row r="1256" spans="1:12" ht="16.2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A1256" s="9">
+        <v>45978</v>
+      </c>
+      <c r="B1256" s="10" t="s">
+        <v>490</v>
+      </c>
+      <c r="C1256" s="10" t="s">
+        <v>355</v>
+      </c>
+      <c r="D1256" s="11" t="s">
+        <v>25</v>
+      </c>
+      <c r="E1256" s="11">
+        <v>-24</v>
+      </c>
+      <c r="F1256" s="11">
+        <v>135.5</v>
+      </c>
+      <c r="G1256" s="11">
+        <v>-10000</v>
+      </c>
+      <c r="H1256" s="11" t="s">
+        <v>1406</v>
+      </c>
+      <c r="I1256" s="11">
+        <v>22</v>
+      </c>
+      <c r="J1256" s="11">
+        <v>-2</v>
+      </c>
+      <c r="K1256" s="11">
+        <v>140</v>
+      </c>
+      <c r="L1256" s="11">
+        <v>4.5</v>
+      </c>
+    </row>
+    <row r="1257" spans="1:12" ht="16.2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A1257" s="12">
+        <v>45978</v>
+      </c>
+      <c r="B1257" s="13" t="s">
+        <v>355</v>
+      </c>
+      <c r="C1257" s="13" t="s">
+        <v>490</v>
+      </c>
+      <c r="D1257" s="14" t="s">
+        <v>23</v>
+      </c>
+      <c r="E1257" s="14">
+        <v>24</v>
+      </c>
+      <c r="F1257" s="14">
+        <v>135.5</v>
+      </c>
+      <c r="G1257" s="14">
+        <v>3000</v>
+      </c>
+      <c r="H1257" s="14" t="s">
+        <v>1407</v>
+      </c>
+      <c r="I1257" s="14">
+        <v>-22</v>
+      </c>
+      <c r="J1257" s="14">
+        <v>2</v>
+      </c>
+      <c r="K1257" s="14">
+        <v>140</v>
+      </c>
+      <c r="L1257" s="14">
+        <v>4.5</v>
+      </c>
+    </row>
+    <row r="1258" spans="1:12" ht="16.2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A1258" s="9">
+        <v>45978</v>
+      </c>
+      <c r="B1258" s="10" t="s">
+        <v>56</v>
+      </c>
+      <c r="C1258" s="10" t="s">
+        <v>376</v>
+      </c>
+      <c r="D1258" s="11" t="s">
+        <v>25</v>
+      </c>
+      <c r="E1258" s="11">
+        <v>-15.5</v>
+      </c>
+      <c r="F1258" s="11">
+        <v>142</v>
+      </c>
+      <c r="G1258" s="11">
+        <v>-1800</v>
+      </c>
+      <c r="H1258" s="11" t="s">
+        <v>1408</v>
+      </c>
+      <c r="I1258" s="11">
+        <v>34</v>
+      </c>
+      <c r="J1258" s="11">
+        <v>18.5</v>
+      </c>
+      <c r="K1258" s="11">
+        <v>134</v>
+      </c>
+      <c r="L1258" s="11">
+        <v>-8</v>
+      </c>
+    </row>
+    <row r="1259" spans="1:12" ht="16.2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A1259" s="12">
+        <v>45978</v>
+      </c>
+      <c r="B1259" s="13" t="s">
+        <v>376</v>
+      </c>
+      <c r="C1259" s="13" t="s">
+        <v>56</v>
+      </c>
+      <c r="D1259" s="14" t="s">
+        <v>23</v>
+      </c>
+      <c r="E1259" s="14">
+        <v>15.5</v>
+      </c>
+      <c r="F1259" s="14">
+        <v>142</v>
+      </c>
+      <c r="G1259" s="14">
+        <v>1000</v>
+      </c>
+      <c r="H1259" s="14" t="s">
+        <v>1409</v>
+      </c>
+      <c r="I1259" s="14">
+        <v>-34</v>
+      </c>
+      <c r="J1259" s="14">
+        <v>-18.5</v>
+      </c>
+      <c r="K1259" s="14">
+        <v>134</v>
+      </c>
+      <c r="L1259" s="14">
+        <v>-8</v>
+      </c>
+    </row>
+    <row r="1260" spans="1:12" ht="16.2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A1260" s="9">
+        <v>45978</v>
+      </c>
+      <c r="B1260" s="10" t="s">
+        <v>188</v>
+      </c>
+      <c r="C1260" s="10" t="s">
+        <v>485</v>
+      </c>
+      <c r="D1260" s="11" t="s">
+        <v>25</v>
+      </c>
+      <c r="E1260" s="11">
+        <v>-35</v>
+      </c>
+      <c r="F1260" s="11">
+        <v>160</v>
+      </c>
+      <c r="G1260" s="11">
+        <v>-10000</v>
+      </c>
+      <c r="H1260" s="11" t="s">
+        <v>1410</v>
+      </c>
+      <c r="I1260" s="11">
+        <v>72</v>
+      </c>
+      <c r="J1260" s="11">
+        <v>37</v>
+      </c>
+      <c r="K1260" s="11">
+        <v>172</v>
+      </c>
+      <c r="L1260" s="11">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="1261" spans="1:12" ht="16.2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A1261" s="12">
+        <v>45978</v>
+      </c>
+      <c r="B1261" s="13" t="s">
+        <v>485</v>
+      </c>
+      <c r="C1261" s="13" t="s">
+        <v>188</v>
+      </c>
+      <c r="D1261" s="14" t="s">
+        <v>23</v>
+      </c>
+      <c r="E1261" s="14">
+        <v>35</v>
+      </c>
+      <c r="F1261" s="14">
+        <v>160</v>
+      </c>
+      <c r="G1261" s="14">
+        <v>3000</v>
+      </c>
+      <c r="H1261" s="14" t="s">
+        <v>1411</v>
+      </c>
+      <c r="I1261" s="14">
+        <v>-72</v>
+      </c>
+      <c r="J1261" s="14">
+        <v>-37</v>
+      </c>
+      <c r="K1261" s="14">
+        <v>172</v>
+      </c>
+      <c r="L1261" s="14">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="1262" spans="1:12" ht="16.2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A1262" s="9">
+        <v>45978</v>
+      </c>
+      <c r="B1262" s="10" t="s">
+        <v>448</v>
+      </c>
+      <c r="C1262" s="10" t="s">
+        <v>432</v>
+      </c>
+      <c r="D1262" s="11" t="s">
+        <v>25</v>
+      </c>
+      <c r="E1262" s="11">
+        <v>-13.5</v>
+      </c>
+      <c r="F1262" s="11">
+        <v>142</v>
+      </c>
+      <c r="G1262" s="11">
+        <v>-1350</v>
+      </c>
+      <c r="H1262" s="11" t="s">
+        <v>442</v>
+      </c>
+      <c r="I1262" s="11">
+        <v>12</v>
+      </c>
+      <c r="J1262" s="11">
+        <v>-1.5</v>
+      </c>
+      <c r="K1262" s="11">
+        <v>162</v>
+      </c>
+      <c r="L1262" s="11">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="1263" spans="1:12" ht="16.2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A1263" s="12">
+        <v>45978</v>
+      </c>
+      <c r="B1263" s="13" t="s">
+        <v>432</v>
+      </c>
+      <c r="C1263" s="13" t="s">
+        <v>448</v>
+      </c>
+      <c r="D1263" s="14" t="s">
+        <v>23</v>
+      </c>
+      <c r="E1263" s="14">
+        <v>13.5</v>
+      </c>
+      <c r="F1263" s="14">
+        <v>142</v>
+      </c>
+      <c r="G1263" s="14">
+        <v>800</v>
+      </c>
+      <c r="H1263" s="14" t="s">
+        <v>441</v>
+      </c>
+      <c r="I1263" s="14">
+        <v>-12</v>
+      </c>
+      <c r="J1263" s="14">
+        <v>1.5</v>
+      </c>
+      <c r="K1263" s="14">
+        <v>162</v>
+      </c>
+      <c r="L1263" s="14">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="1264" spans="1:12" ht="16.2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A1264" s="9">
+        <v>45978</v>
+      </c>
+      <c r="B1264" s="10" t="s">
+        <v>238</v>
+      </c>
+      <c r="C1264" s="10" t="s">
+        <v>245</v>
+      </c>
+      <c r="D1264" s="11" t="s">
+        <v>25</v>
+      </c>
+      <c r="E1264" s="11">
+        <v>-13.5</v>
+      </c>
+      <c r="F1264" s="11">
+        <v>162.5</v>
+      </c>
+      <c r="G1264" s="11">
+        <v>-1400</v>
+      </c>
+      <c r="H1264" s="11" t="s">
+        <v>1061</v>
+      </c>
+      <c r="I1264" s="11">
+        <v>4</v>
+      </c>
+      <c r="J1264" s="11">
+        <v>-9.5</v>
+      </c>
+      <c r="K1264" s="11">
+        <v>170</v>
+      </c>
+      <c r="L1264" s="11">
+        <v>7.5</v>
+      </c>
+    </row>
+    <row r="1265" spans="1:12" ht="16.2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A1265" s="12">
+        <v>45978</v>
+      </c>
+      <c r="B1265" s="13" t="s">
+        <v>245</v>
+      </c>
+      <c r="C1265" s="13" t="s">
+        <v>238</v>
+      </c>
+      <c r="D1265" s="14" t="s">
+        <v>23</v>
+      </c>
+      <c r="E1265" s="14">
+        <v>13.5</v>
+      </c>
+      <c r="F1265" s="14">
+        <v>162.5</v>
+      </c>
+      <c r="G1265" s="14">
+        <v>836</v>
+      </c>
+      <c r="H1265" s="14" t="s">
+        <v>1060</v>
+      </c>
+      <c r="I1265" s="14">
+        <v>-4</v>
+      </c>
+      <c r="J1265" s="14">
+        <v>9.5</v>
+      </c>
+      <c r="K1265" s="14">
+        <v>170</v>
+      </c>
+      <c r="L1265" s="14">
+        <v>7.5</v>
+      </c>
+    </row>
+    <row r="1266" spans="1:12" ht="16.2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A1266" s="9">
+        <v>45978</v>
+      </c>
+      <c r="B1266" s="10" t="s">
+        <v>229</v>
+      </c>
+      <c r="C1266" s="10" t="s">
+        <v>391</v>
+      </c>
+      <c r="D1266" s="11" t="s">
+        <v>25</v>
+      </c>
+      <c r="E1266" s="11">
+        <v>-4</v>
+      </c>
+      <c r="F1266" s="11">
+        <v>152.5</v>
+      </c>
+      <c r="G1266" s="11">
+        <v>-185</v>
+      </c>
+      <c r="H1266" s="11" t="s">
+        <v>1186</v>
+      </c>
+      <c r="I1266" s="11">
+        <v>-2</v>
+      </c>
+      <c r="J1266" s="11">
+        <v>-6</v>
+      </c>
+      <c r="K1266" s="11">
+        <v>120</v>
+      </c>
+      <c r="L1266" s="11">
+        <v>-32.5</v>
+      </c>
+    </row>
+    <row r="1267" spans="1:12" ht="16.2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A1267" s="12">
+        <v>45978</v>
+      </c>
+      <c r="B1267" s="13" t="s">
+        <v>391</v>
+      </c>
+      <c r="C1267" s="13" t="s">
+        <v>229</v>
+      </c>
+      <c r="D1267" s="14" t="s">
+        <v>23</v>
+      </c>
+      <c r="E1267" s="14">
+        <v>4</v>
+      </c>
+      <c r="F1267" s="14">
+        <v>152.5</v>
+      </c>
+      <c r="G1267" s="14">
+        <v>154</v>
+      </c>
+      <c r="H1267" s="14" t="s">
+        <v>1185</v>
+      </c>
+      <c r="I1267" s="14">
+        <v>2</v>
+      </c>
+      <c r="J1267" s="14">
+        <v>6</v>
+      </c>
+      <c r="K1267" s="14">
+        <v>120</v>
+      </c>
+      <c r="L1267" s="14">
+        <v>-32.5</v>
+      </c>
+    </row>
+    <row r="1268" spans="1:12" ht="16.2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A1268" s="9">
+        <v>45978</v>
+      </c>
+      <c r="B1268" s="10" t="s">
+        <v>276</v>
+      </c>
+      <c r="C1268" s="10" t="s">
+        <v>667</v>
+      </c>
+      <c r="D1268" s="11" t="s">
+        <v>25</v>
+      </c>
+      <c r="E1268" s="11">
+        <v>-25.5</v>
+      </c>
+      <c r="F1268" s="11">
+        <v>147</v>
+      </c>
+      <c r="G1268" s="11">
+        <v>-6500</v>
+      </c>
+      <c r="H1268" s="11" t="s">
+        <v>1412</v>
+      </c>
+      <c r="I1268" s="11">
+        <v>25</v>
+      </c>
+      <c r="J1268" s="11">
+        <v>-0.5</v>
+      </c>
+      <c r="K1268" s="11">
+        <v>163</v>
+      </c>
+      <c r="L1268" s="11">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="1269" spans="1:12" ht="16.2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A1269" s="12">
+        <v>45978</v>
+      </c>
+      <c r="B1269" s="13" t="s">
+        <v>667</v>
+      </c>
+      <c r="C1269" s="13" t="s">
+        <v>276</v>
+      </c>
+      <c r="D1269" s="14" t="s">
+        <v>23</v>
+      </c>
+      <c r="E1269" s="14">
+        <v>25.5</v>
+      </c>
+      <c r="F1269" s="14">
+        <v>147</v>
+      </c>
+      <c r="G1269" s="14">
+        <v>2000</v>
+      </c>
+      <c r="H1269" s="14" t="s">
+        <v>1413</v>
+      </c>
+      <c r="I1269" s="14">
+        <v>-25</v>
+      </c>
+      <c r="J1269" s="14">
+        <v>0.5</v>
+      </c>
+      <c r="K1269" s="14">
+        <v>163</v>
+      </c>
+      <c r="L1269" s="14">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="1270" spans="1:12" ht="16.2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A1270" s="9">
+        <v>45978</v>
+      </c>
+      <c r="B1270" s="10" t="s">
+        <v>303</v>
+      </c>
+      <c r="C1270" s="10" t="s">
+        <v>772</v>
+      </c>
+      <c r="D1270" s="11" t="s">
+        <v>25</v>
+      </c>
+      <c r="E1270" s="11">
+        <v>-34.5</v>
+      </c>
+      <c r="F1270" s="11">
+        <v>166.5</v>
+      </c>
+      <c r="G1270" s="11">
+        <v>-10000</v>
+      </c>
+      <c r="H1270" s="11" t="s">
+        <v>1318</v>
+      </c>
+      <c r="I1270" s="11">
+        <v>18</v>
+      </c>
+      <c r="J1270" s="11">
+        <v>-16.5</v>
+      </c>
+      <c r="K1270" s="11">
+        <v>164</v>
+      </c>
+      <c r="L1270" s="11">
+        <v>-2.5</v>
+      </c>
+    </row>
+    <row r="1271" spans="1:12" ht="16.2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A1271" s="12">
+        <v>45978</v>
+      </c>
+      <c r="B1271" s="13" t="s">
+        <v>772</v>
+      </c>
+      <c r="C1271" s="13" t="s">
+        <v>303</v>
+      </c>
+      <c r="D1271" s="14" t="s">
+        <v>23</v>
+      </c>
+      <c r="E1271" s="14">
+        <v>34.5</v>
+      </c>
+      <c r="F1271" s="14">
+        <v>166.5</v>
+      </c>
+      <c r="G1271" s="14">
+        <v>3300</v>
+      </c>
+      <c r="H1271" s="14" t="s">
+        <v>1317</v>
+      </c>
+      <c r="I1271" s="14">
+        <v>-18</v>
+      </c>
+      <c r="J1271" s="14">
+        <v>16.5</v>
+      </c>
+      <c r="K1271" s="14">
+        <v>164</v>
+      </c>
+      <c r="L1271" s="14">
+        <v>-2.5</v>
+      </c>
+    </row>
+    <row r="1272" spans="1:12" ht="16.2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A1272" s="9">
+        <v>45978</v>
+      </c>
+      <c r="B1272" s="10" t="s">
+        <v>644</v>
+      </c>
+      <c r="C1272" s="10" t="s">
+        <v>315</v>
+      </c>
+      <c r="D1272" s="11" t="s">
+        <v>25</v>
+      </c>
+      <c r="E1272" s="11">
+        <v>-7.5</v>
+      </c>
+      <c r="F1272" s="11">
+        <v>153.5</v>
+      </c>
+      <c r="G1272" s="11">
+        <v>-310</v>
+      </c>
+      <c r="H1272" s="11" t="s">
+        <v>1414</v>
+      </c>
+      <c r="I1272" s="11">
+        <v>-9</v>
+      </c>
+      <c r="J1272" s="11">
+        <v>-16.5</v>
+      </c>
+      <c r="K1272" s="11">
+        <v>133</v>
+      </c>
+      <c r="L1272" s="11">
+        <v>-20.5</v>
+      </c>
+    </row>
+    <row r="1273" spans="1:12" ht="16.2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A1273" s="12">
+        <v>45978</v>
+      </c>
+      <c r="B1273" s="13" t="s">
+        <v>315</v>
+      </c>
+      <c r="C1273" s="13" t="s">
+        <v>644</v>
+      </c>
+      <c r="D1273" s="14" t="s">
+        <v>23</v>
+      </c>
+      <c r="E1273" s="14">
+        <v>7.5</v>
+      </c>
+      <c r="F1273" s="14">
+        <v>153.5</v>
+      </c>
+      <c r="G1273" s="14">
+        <v>250</v>
+      </c>
+      <c r="H1273" s="14" t="s">
+        <v>1415</v>
+      </c>
+      <c r="I1273" s="14">
+        <v>9</v>
+      </c>
+      <c r="J1273" s="14">
+        <v>16.5</v>
+      </c>
+      <c r="K1273" s="14">
+        <v>133</v>
+      </c>
+      <c r="L1273" s="14">
+        <v>-20.5</v>
+      </c>
+    </row>
+    <row r="1274" spans="1:12" ht="16.2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A1274" s="9">
+        <v>45978</v>
+      </c>
+      <c r="B1274" s="10" t="s">
+        <v>211</v>
+      </c>
+      <c r="C1274" s="10" t="s">
+        <v>969</v>
+      </c>
+      <c r="D1274" s="11" t="s">
+        <v>25</v>
+      </c>
+      <c r="E1274" s="11">
+        <v>10.5</v>
+      </c>
+      <c r="F1274" s="11">
+        <v>140.5</v>
+      </c>
+      <c r="G1274" s="11">
+        <v>410</v>
+      </c>
+      <c r="H1274" s="11" t="s">
+        <v>1416</v>
+      </c>
+      <c r="I1274" s="11">
+        <v>-13</v>
+      </c>
+      <c r="J1274" s="11">
+        <v>-2.5</v>
+      </c>
+      <c r="K1274" s="11">
+        <v>145</v>
+      </c>
+      <c r="L1274" s="11">
+        <v>4.5</v>
+      </c>
+    </row>
+    <row r="1275" spans="1:12" ht="16.2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A1275" s="15">
+        <v>45978</v>
+      </c>
+      <c r="B1275" s="16" t="s">
+        <v>969</v>
+      </c>
+      <c r="C1275" s="16" t="s">
+        <v>211</v>
+      </c>
+      <c r="D1275" s="17" t="s">
+        <v>23</v>
+      </c>
+      <c r="E1275" s="17">
+        <v>-10.5</v>
+      </c>
+      <c r="F1275" s="17">
+        <v>140.5</v>
+      </c>
+      <c r="G1275" s="17">
+        <v>-550</v>
+      </c>
+      <c r="H1275" s="17" t="s">
+        <v>1417</v>
+      </c>
+      <c r="I1275" s="17">
+        <v>13</v>
+      </c>
+      <c r="J1275" s="17">
+        <v>2.5</v>
+      </c>
+      <c r="K1275" s="17">
+        <v>145</v>
+      </c>
+      <c r="L1275" s="17">
+        <v>4.5</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>